<commit_message>
Some cleanups. Added verbosity control for messages and plotting.
</commit_message>
<xml_diff>
--- a/radium_log.xlsx
+++ b/radium_log.xlsx
@@ -1,81 +1,45 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bub8ga\radex\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="radium" sheetId="1" r:id="rId1"/>
+    <sheet name="radium" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <definedNames/>
+  <calcPr calcId="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="9">
-  <si>
-    <t>DATO</t>
-  </si>
-  <si>
-    <t>SERIE</t>
-  </si>
-  <si>
-    <t>MDA [Bq]</t>
-  </si>
-  <si>
-    <t>Følsomhed [cps/Bq]</t>
-  </si>
-  <si>
-    <t>Aktivitet [Bq]</t>
-  </si>
-  <si>
-    <t>Dage til bortskaffelse</t>
-  </si>
-  <si>
-    <t>Dato for bortskaffelse</t>
-  </si>
-  <si>
-    <t>Dato for registrering</t>
-  </si>
-  <si>
-    <t>-</t>
-  </si>
-</sst>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd"/>
     <numFmt numFmtId="165" formatCode="yyyy/mm/dd;@"/>
+    <numFmt numFmtId="166" formatCode="yyyy-mm-dd"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="2">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <b val="1"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -93,27 +57,87 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+  <cellXfs count="7">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -379,78 +403,170 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:H4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="2" width="20.5703125" style="4" customWidth="1"/>
-    <col min="3" max="3" width="15.7109375" style="4" customWidth="1"/>
-    <col min="4" max="4" width="20.5703125" style="4" customWidth="1"/>
-    <col min="5" max="5" width="15.5703125" style="4" customWidth="1"/>
-    <col min="6" max="6" width="21.5703125" style="4" customWidth="1"/>
-    <col min="7" max="7" width="22.5703125" style="2" customWidth="1"/>
-    <col min="8" max="8" width="23.85546875" style="5" customWidth="1"/>
+    <col width="20.5703125" customWidth="1" style="4" min="1" max="2"/>
+    <col width="15.7109375" customWidth="1" style="4" min="3" max="3"/>
+    <col width="20.5703125" customWidth="1" style="4" min="4" max="4"/>
+    <col width="15.5703125" customWidth="1" style="4" min="5" max="5"/>
+    <col width="21.5703125" customWidth="1" style="4" min="6" max="6"/>
+    <col width="22.5703125" customWidth="1" style="2" min="7" max="7"/>
+    <col width="23.85546875" customWidth="1" style="5" min="8" max="8"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="5" t="s">
-        <v>7</v>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>DATO</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>SERIE</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>MDA [Bq]</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>Følsomhed [cps/Bq]</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>Aktivitet [Bq]</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>Dage til bortskaffelse</t>
+        </is>
+      </c>
+      <c r="G1" s="2" t="inlineStr">
+        <is>
+          <t>Dato for bortskaffelse</t>
+        </is>
+      </c>
+      <c r="H1" s="5" t="inlineStr">
+        <is>
+          <t>Dato for registrering</t>
+        </is>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E2" t="s">
-        <v>8</v>
-      </c>
-      <c r="F2" t="s">
-        <v>8</v>
-      </c>
-      <c r="G2" t="s">
-        <v>8</v>
-      </c>
-      <c r="H2" s="5" t="s">
-        <v>8</v>
+    <row r="2">
+      <c r="A2" s="3" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="B2" s="3" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H2" s="5" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="6" t="n">
+        <v>44421</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="C3" t="n">
+        <v>32.91409991687141</v>
+      </c>
+      <c r="D3" t="n">
+        <v>0.1983327583213161</v>
+      </c>
+      <c r="E3" t="n">
+        <v>79067.23346841783</v>
+      </c>
+      <c r="F3" t="n">
+        <v>91.67849944186584</v>
+      </c>
+      <c r="G3" s="6" t="n">
+        <v>44512</v>
+      </c>
+      <c r="H3" s="6" t="n">
+        <v>44481</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="6" t="n">
+        <v>44421</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>7</t>
+        </is>
+      </c>
+      <c r="C4" t="n">
+        <v>32.91409991687141</v>
+      </c>
+      <c r="D4" t="n">
+        <v>0.1983327583213161</v>
+      </c>
+      <c r="E4" t="n">
+        <v>13243.20223981312</v>
+      </c>
+      <c r="F4" t="n">
+        <v>62.29126098790209</v>
+      </c>
+      <c r="G4" s="6" t="n">
+        <v>44483</v>
+      </c>
+      <c r="H4" s="6" t="n">
+        <v>44481</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait"/>
+  <pageSetup orientation="portrait" paperSize="9"/>
 </worksheet>
 </file>
</xml_diff>